<commit_message>
Address update / Inventory start
</commit_message>
<xml_diff>
--- a/PO_Template.xlsx
+++ b/PO_Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F314989D-EF40-4CF9-86A1-C27B5882A464}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEB712F-33C2-4D6D-8274-3A37726A2A2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2925" yWindow="3570" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1470" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="2" r:id="rId1"/>
@@ -102,12 +102,6 @@
     <t>Orlando Florida, 32819</t>
   </si>
   <si>
-    <t>7061 Grand National Drive</t>
-  </si>
-  <si>
-    <t>Suite 107A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quote:  </t>
   </si>
   <si>
@@ -144,7 +138,13 @@
     <t>PART DESCRIPTION</t>
   </si>
   <si>
-    <t>7061 Grand National Dr. Suite 107A</t>
+    <t>7041 Grand National Dr. Suite 100</t>
+  </si>
+  <si>
+    <t>7041 Grand National Drive</t>
+  </si>
+  <si>
+    <t>Suite 100</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,7 +991,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -1109,6 +1115,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1121,12 +1143,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1139,14 +1155,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1717,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1768,10 +1780,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="13"/>
+      <c r="B4" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="56"/>
       <c r="D4" s="13"/>
       <c r="E4" s="19"/>
       <c r="F4" s="2"/>
@@ -1864,7 +1876,7 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
@@ -1873,7 +1885,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H10" s="37"/>
       <c r="I10" s="13"/>
@@ -1882,20 +1894,20 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="D11" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="57"/>
       <c r="F11" s="7"/>
       <c r="G11" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="38">
         <f ca="1">TODAY()</f>
-        <v>43549</v>
+        <v>43564</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="1"/>
@@ -1905,16 +1917,16 @@
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="D12" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="57"/>
       <c r="F12" s="7"/>
       <c r="G12" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="13"/>
@@ -1928,7 +1940,7 @@
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -1937,7 +1949,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H13" s="39"/>
       <c r="I13" s="13"/>
@@ -1950,14 +1962,14 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="13"/>
@@ -2022,10 +2034,10 @@
     <row r="18" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="54"/>
+      <c r="C18" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="44"/>
       <c r="E18" s="10">
         <v>0</v>
       </c>
@@ -2038,22 +2050,22 @@
         <v>0</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="48"/>
+      <c r="C19" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="46"/>
       <c r="E19" s="10"/>
       <c r="F19" s="34"/>
       <c r="G19" s="4"/>
@@ -2062,22 +2074,22 @@
         <v/>
       </c>
       <c r="I19" s="2"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="43"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="48"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="46"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="4"/>
@@ -2091,7 +2103,7 @@
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="47"/>
-      <c r="D21" s="48"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="4"/>
@@ -2106,7 +2118,7 @@
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="4"/>
@@ -2121,7 +2133,7 @@
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="4"/>
@@ -2136,7 +2148,7 @@
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
+      <c r="D24" s="46"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="4"/>
@@ -2151,7 +2163,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="4"/>
@@ -2168,7 +2180,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="4"/>
@@ -2183,7 +2195,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="4"/>
@@ -2197,7 +2209,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="D28" s="46"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="4"/>
@@ -2211,7 +2223,7 @@
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="47"/>
-      <c r="D29" s="48"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="4"/>
@@ -2225,7 +2237,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="47"/>
-      <c r="D30" s="48"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="4"/>
@@ -2239,7 +2251,7 @@
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="47"/>
-      <c r="D31" s="48"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="4"/>
@@ -2253,7 +2265,7 @@
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
+      <c r="D32" s="46"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="4"/>
@@ -2268,7 +2280,7 @@
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="47"/>
-      <c r="D33" s="48"/>
+      <c r="D33" s="46"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="4"/>
@@ -2283,7 +2295,7 @@
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="4"/>
@@ -2298,7 +2310,7 @@
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="47"/>
-      <c r="D35" s="48"/>
+      <c r="D35" s="46"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="4"/>
@@ -2313,7 +2325,7 @@
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="47"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="4"/>
@@ -2328,7 +2340,7 @@
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="47"/>
-      <c r="D37" s="48"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="4"/>
@@ -2343,7 +2355,7 @@
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="4"/>
@@ -2358,7 +2370,7 @@
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="47"/>
-      <c r="D39" s="48"/>
+      <c r="D39" s="46"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="4"/>
@@ -2373,7 +2385,7 @@
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="47"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="46"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="4"/>
@@ -2388,7 +2400,7 @@
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="47"/>
-      <c r="D41" s="48"/>
+      <c r="D41" s="46"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="4"/>
@@ -2402,8 +2414,8 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="33"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="50"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
       <c r="G42" s="5"/>
@@ -2446,9 +2458,9 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
       <c r="E45" s="12"/>
       <c r="F45" s="2"/>
       <c r="G45" s="6"/>
@@ -2458,8 +2470,8 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="47"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="9"/>
       <c r="F46" s="2"/>
       <c r="G46" s="6" t="s">
@@ -2486,8 +2498,8 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="47"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
       <c r="E48" s="9"/>
       <c r="F48" s="2"/>
       <c r="G48" s="6"/>
@@ -2496,9 +2508,9 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="11"/>
       <c r="F49" s="2"/>
       <c r="G49" s="6"/>
@@ -2507,9 +2519,9 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -2604,21 +2616,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
     <mergeCell ref="K18:R19"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:D50"/>
@@ -2635,6 +2632,21 @@
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B48:D48"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>